<commit_message>
La barre de recherche est fonctionnelle dans la vue.
</commit_message>
<xml_diff>
--- a/Classeur1.xlsx
+++ b/Classeur1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthieu/Workspace/java-workspaces/cgi010-reunion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6893E76-D9C2-2F4A-9A10-3505CDFABCBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F90985-6A2D-3B47-85BB-2EF022BCC720}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="440" windowWidth="30760" windowHeight="20360" xr2:uid="{7878FE48-B459-3546-9F57-303F83442CA7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Backlog projet Re-Union</t>
   </si>
@@ -163,13 +163,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,16 +206,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
@@ -235,11 +232,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -615,7 +654,7 @@
   <dimension ref="A2:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,46 +672,46 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="10"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="12">
         <v>2</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="12">
         <v>10</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="12">
         <f>QUOTIENT(C7, B7)</f>
         <v>5</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -690,7 +729,7 @@
         <f t="shared" ref="D8:D25" si="0">C8/B8</f>
         <v>1</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -699,68 +738,68 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="11"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12">
         <v>10</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3">
-        <v>1</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="B12" s="12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="12">
         <v>8</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3">
-        <v>1</v>
-      </c>
-      <c r="C13" s="3">
+      <c r="B13" s="12">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12">
         <v>8</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -778,7 +817,7 @@
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="E14" s="9"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
@@ -794,7 +833,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E15" s="9"/>
+      <c r="E15" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -810,30 +851,30 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E16" s="9"/>
+      <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="9"/>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="9"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="11"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -849,7 +890,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
@@ -865,23 +906,23 @@
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E21" s="9"/>
+      <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="11"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -897,23 +938,25 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E24" s="9"/>
+      <c r="E24" s="8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="3">
-        <v>1</v>
-      </c>
-      <c r="C25" s="3">
+      <c r="B25" s="13">
+        <v>1</v>
+      </c>
+      <c r="C25" s="13">
         <v>5</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="13">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -922,8 +965,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E7:E25">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",E7)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"OK"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>